<commit_message>
finish import aphid traits -still issues with judith indiv
</commit_message>
<xml_diff>
--- a/data/Checklist 2020.xlsx
+++ b/data/Checklist 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\PROJEKT-ARBEIT\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maud/Dropbox/Work/doc boulot/postdoc Berlin/R projects/AphidTraits/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E39C8C-8D5D-46ED-BC50-75C74CB56EB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA07A38-045A-C04D-AC5F-C778B07C4B68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="3" xr2:uid="{83007F86-AA6F-4A3C-9AE4-7210E3AB2052}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24500" windowHeight="15500" xr2:uid="{83007F86-AA6F-4A3C-9AE4-7210E3AB2052}"/>
   </bookViews>
   <sheets>
     <sheet name="Oh_01" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,6 @@
     <sheet name="Spandau R2 6.8.19" sheetId="18" r:id="rId21"/>
     <sheet name="Nordbahnhof U1 30.8.19" sheetId="17" r:id="rId22"/>
     <sheet name="Südgelände U3 7.8.19" sheetId="19" r:id="rId23"/>
-    <sheet name="Tabelle2" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -436,7 +435,7 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,7 +451,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -750,18 +749,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF0A5DB-A781-4832-96C4-9796ADDFE949}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="15.6328125" customWidth="1"/>
-    <col min="11" max="11" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -840,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -875,7 +874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -909,7 +908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -947,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -985,7 +984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -997,7 +996,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1032,7 +1031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -1138,7 +1137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -1156,7 +1155,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1168,7 +1167,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -1308,7 +1307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -1346,7 +1345,7 @@
         <v>44130</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1358,7 +1357,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -1434,7 +1433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>4</v>
       </c>
@@ -1472,7 +1471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>4</v>
       </c>
@@ -1551,10 +1550,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M25" s="11"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>75</v>
       </c>
@@ -1589,7 +1588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>75</v>
       </c>
@@ -1624,11 +1623,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>76</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>76</v>
       </c>
@@ -1698,7 +1697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>77</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
         <v>77</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>77</v>
       </c>
@@ -1821,9 +1820,9 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1940,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1994,9 +1993,9 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2180,7 +2179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2229,9 +2228,9 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2272,7 +2271,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2351,7 +2350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2402,9 +2401,9 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2445,7 +2444,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2480,7 +2479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2585,7 +2584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2633,9 +2632,9 @@
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2676,7 +2675,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2781,7 +2780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2867,9 +2866,9 @@
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3056,7 +3055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3107,9 +3106,9 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3150,7 +3149,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3185,7 +3184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3258,7 +3257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3293,7 +3292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L7" s="10"/>
     </row>
   </sheetData>
@@ -3347,9 +3346,9 @@
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3403,9 +3402,9 @@
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3446,7 +3445,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3522,7 +3521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3601,7 +3600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3652,9 +3651,9 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3695,7 +3694,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3730,7 +3729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3765,7 +3764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3800,7 +3799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3835,7 +3834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3883,13 +3882,13 @@
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3930,7 +3929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3971,7 +3970,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -4053,7 +4052,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4094,7 +4093,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -4135,7 +4134,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -4145,7 +4144,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -4223,7 +4222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -4262,7 +4261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -4300,7 +4299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -4339,7 +4338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4349,7 +4348,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -4390,7 +4389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -4429,7 +4428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -4468,7 +4467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -4509,7 +4508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -4548,7 +4547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4558,7 +4557,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -4596,7 +4595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -4634,7 +4633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>4</v>
       </c>
@@ -4675,7 +4674,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -4716,7 +4715,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>4</v>
       </c>
@@ -4757,7 +4756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4767,7 +4766,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>5</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>5</v>
       </c>
@@ -4846,7 +4845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>5</v>
       </c>
@@ -4884,7 +4883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>5</v>
       </c>
@@ -4922,7 +4921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>5</v>
       </c>
@@ -4978,9 +4977,9 @@
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5021,7 +5020,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5059,7 +5058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5097,7 +5096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5135,7 +5134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5224,9 +5223,9 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5267,7 +5266,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5302,7 +5301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5337,7 +5336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5372,7 +5371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5407,7 +5406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5455,9 +5454,9 @@
       <selection activeCell="L2" sqref="L2:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5498,7 +5497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5533,7 +5532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5568,7 +5567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5638,7 +5637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5683,12 +5682,12 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5729,7 +5728,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5764,7 +5763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5799,7 +5798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5834,7 +5833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5869,7 +5868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5905,18 +5904,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66D2DAB-C910-45FF-97AC-151497CF1BA1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5929,13 +5916,13 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5976,7 +5963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6014,7 +6001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6055,7 +6042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -6096,7 +6083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -6134,7 +6121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -6173,7 +6160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6183,7 +6170,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -6224,7 +6211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -6265,7 +6252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -6303,7 +6290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -6341,7 +6328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -6385,7 +6372,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6395,7 +6382,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -6436,7 +6423,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>5</v>
       </c>
@@ -6477,7 +6464,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>5</v>
       </c>
@@ -6518,7 +6505,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>5</v>
       </c>
@@ -6559,7 +6546,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -6614,16 +6601,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B236D52-03BE-44BA-974D-DC97A5A50958}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6664,7 +6651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6705,7 +6692,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6747,7 +6734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -6788,7 +6775,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -6829,7 +6816,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -6870,7 +6857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -6923,12 +6910,12 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6969,7 +6956,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -7007,7 +6994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -7045,7 +7032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -7084,7 +7071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -7122,7 +7109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -7160,7 +7147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -7170,7 +7157,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -7211,7 +7198,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -7252,7 +7239,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -7293,7 +7280,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -7334,7 +7321,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -7375,7 +7362,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -7385,7 +7372,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -7423,7 +7410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>5</v>
       </c>
@@ -7461,7 +7448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>5</v>
       </c>
@@ -7499,7 +7486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>5</v>
       </c>
@@ -7537,7 +7524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -7593,14 +7580,14 @@
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7641,7 +7628,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -7682,7 +7669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -7720,7 +7707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -7764,7 +7751,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -7805,7 +7792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -7849,7 +7836,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -7859,7 +7846,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -7900,7 +7887,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -7941,7 +7928,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -7982,7 +7969,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -8023,7 +8010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -8064,7 +8051,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -8074,7 +8061,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -8115,7 +8102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -8153,7 +8140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -8194,7 +8181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -8235,7 +8222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -8273,7 +8260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>77</v>
       </c>
@@ -8308,7 +8295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>77</v>
       </c>
@@ -8343,7 +8330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>77</v>
       </c>
@@ -8378,7 +8365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>77</v>
       </c>
@@ -8428,17 +8415,17 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8479,7 +8466,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -8517,7 +8504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -8555,7 +8542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -8593,7 +8580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -8631,7 +8618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -8669,7 +8656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -8679,7 +8666,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -8717,7 +8704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -8755,7 +8742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -8793,7 +8780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -8831,7 +8818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -8869,7 +8856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -8879,7 +8866,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -8920,7 +8907,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -8961,7 +8948,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -9002,7 +8989,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -9043,7 +9030,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -9084,7 +9071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -9094,7 +9081,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -9129,7 +9116,7 @@
         <v>44132</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -9167,7 +9154,7 @@
         <v>44132</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>4</v>
       </c>
@@ -9205,7 +9192,7 @@
         <v>44132</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -9243,7 +9230,7 @@
         <v>44132</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>4</v>
       </c>
@@ -9278,7 +9265,7 @@
         <v>44132</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -9288,7 +9275,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>5</v>
       </c>
@@ -9332,7 +9319,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>5</v>
       </c>
@@ -9373,7 +9360,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>5</v>
       </c>
@@ -9414,7 +9401,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>5</v>
       </c>
@@ -9455,7 +9442,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>5</v>
       </c>
@@ -9496,7 +9483,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>73</v>
       </c>
@@ -9531,7 +9518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>73</v>
       </c>
@@ -9566,7 +9553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>73</v>
       </c>
@@ -9601,7 +9588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>73</v>
       </c>
@@ -9636,7 +9623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>73</v>
       </c>
@@ -9692,9 +9679,9 @@
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9735,7 +9722,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9770,7 +9757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -9805,7 +9792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -9840,7 +9827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -9875,7 +9862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -9923,9 +9910,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9966,7 +9953,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10001,7 +9988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -10036,7 +10023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -10071,7 +10058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -10106,7 +10093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -10141,7 +10128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -10176,7 +10163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -10211,7 +10198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -10246,7 +10233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -10284,7 +10271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -10319,7 +10306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -10354,7 +10341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -10389,7 +10376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -10427,7 +10414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -10465,7 +10452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>

</xml_diff>